<commit_message>
final changes for part 2
</commit_message>
<xml_diff>
--- a/data/reference-tables/data_dictionary_status_and_trends_dataset.csv.xlsx
+++ b/data/reference-tables/data_dictionary_status_and_trends_dataset.csv.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/63117abe423e2d96/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/63117abe423e2d96/Desktop/INST414/inst414-final-project-Jillian-Conway/data/reference-tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C37F65C8-87D4-40A4-B0C4-0784CC230611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{C37F65C8-87D4-40A4-B0C4-0784CC230611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D166E92C-A10A-4DAE-A17A-6BBADABCB3C5}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="17460" windowHeight="10260" xr2:uid="{75B88FCA-A76E-46CD-AD49-FAF48612EA57}"/>
   </bookViews>
@@ -600,11 +600,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57D4AA7-CBF3-4DB2-80B1-BCCB4622756A}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="25.40625" customWidth="1"/>
+    <col min="2" max="2" width="27.7265625" customWidth="1"/>
+    <col min="3" max="3" width="21.26953125" customWidth="1"/>
+    <col min="4" max="4" width="21.31640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A1" t="s">

</xml_diff>